<commit_message>
- check R-Tools BEFORE installing the packages from CRAN - Use pkgbuild::has_rtools() for checking for Rtools - Add purrr for installation - Add argument 'lib' to installation scripts - Extend vignettes for standard workflow
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/ModelParameters.xlsx
+++ b/tests/data/TestProject/Parameters/ModelParameters.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esqlabs.sharepoint.com/sites/Services/Freigegebene Dokumente/_Project_template_V02.00/WP1_V00.01/Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1541" documentId="13_ncr:1_{4B2F205E-FEDC-4EE6-8C1F-DD0552DF0F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFB32157-80B9-406D-81EE-7DB94DF175FD}"/>
+  <xr:revisionPtr revIDLastSave="1550" documentId="13_ncr:1_{4B2F205E-FEDC-4EE6-8C1F-DD0552DF0F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C3F8D02-8689-4DA2-88B4-3EB0BC12FE16}"/>
   <bookViews>
-    <workbookView xWindow="9190" yWindow="430" windowWidth="28800" windowHeight="15290" tabRatio="976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22282" yWindow="727" windowWidth="24038" windowHeight="13133" tabRatio="976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="5" r:id="rId1"/>
+    <sheet name="Aciclovir" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>Container Path</t>
   </si>
@@ -55,6 +56,12 @@
   </si>
   <si>
     <t>Log Units</t>
+  </si>
+  <si>
+    <t>EHC continuous fraction</t>
+  </si>
+  <si>
+    <t>Organism|Liver</t>
   </si>
 </sst>
 </file>
@@ -387,18 +394,18 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="71.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -412,34 +419,74 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3">
-        <v>-0.1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D10" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{003F998E-5869-417D-A696-38B00449383B}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -681,15 +728,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
@@ -700,23 +738,49 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDADFA4D-689E-4192-9812-F7D7F3DFE5E7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDADFA4D-689E-4192-9812-F7D7F3DFE5E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D118C015-E179-46FB-B6E8-2D926D65EB7E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{253E2BCE-BEE3-46CA-82C7-E211846F5250}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D118C015-E179-46FB-B6E8-2D926D65EB7E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>